<commit_message>
Message sets are on the waay!!
Reading parameters per message/es/trafficSource and writing to ini is about to be completed.
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\pythonProjects\AFDX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\Github\ANCAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD3F13A-C71C-44DE-9399-E0B003DBF85F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E6990E-1407-4320-8A02-F89DD6D6EE5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2184" yWindow="3264" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{60116E78-B1B7-4F11-A25A-D1AE9DCDD0BC}"/>
+    <workbookView xWindow="13968" yWindow="492" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="3" xr2:uid="{60116E78-B1B7-4F11-A25A-D1AE9DCDD0BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
     <sheet name="Topology" sheetId="1" r:id="rId2"/>
+    <sheet name="Settings" sheetId="3" r:id="rId3"/>
+    <sheet name="End Systems" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="92">
   <si>
     <t>ES1</t>
   </si>
@@ -92,8 +94,39 @@
     <t>Exit</t>
   </si>
   <si>
+    <t xml:space="preserve">! Her bağlantı bir kere </t>
+  </si>
+  <si>
+    <t>! Switch'e giren toplam sayı 24'ü geçmeyecek kontrolü</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Define conections. </t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Define conections. </t>
+      <t xml:space="preserve">column </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Entry</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Entry of the connections, column </t>
     </r>
     <r>
       <rPr>
@@ -115,37 +148,225 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> the nodes in A are connected to the</t>
+      <t>: Exit of the connections</t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Entry</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> B</t>
-    </r>
+  </si>
+  <si>
+    <t>x: iki basamaklı olursa</t>
+  </si>
+  <si>
+    <t>Switch Tech Delay</t>
+  </si>
+  <si>
+    <t>4us</t>
+  </si>
+  <si>
+    <t>32us</t>
+  </si>
+  <si>
+    <t>Ethernet Speed</t>
+  </si>
+  <si>
+    <t>Ethernet Cable Length</t>
+  </si>
+  <si>
+    <t>10Mbps</t>
+  </si>
+  <si>
+    <t>100Mbps</t>
+  </si>
+  <si>
+    <t>10m</t>
+  </si>
+  <si>
+    <t>10ms</t>
+  </si>
+  <si>
+    <t>1s</t>
+  </si>
+  <si>
+    <t>0s</t>
+  </si>
+  <si>
+    <t>uniform(0, 5ms)</t>
+  </si>
+  <si>
+    <t>1ms</t>
+  </si>
+  <si>
+    <t>vlid range kontrol</t>
+  </si>
+  <si>
+    <t>S = payload + AFDX Overhead(47B) + PHY Overhead(20B)</t>
+  </si>
+  <si>
+    <t>Sheet: End Systems</t>
+  </si>
+  <si>
+    <t>Define ES parameters and message set</t>
+  </si>
+  <si>
+    <t>uniform içi format kontrolü</t>
+  </si>
+  <si>
+    <t>0x100</t>
+  </si>
+  <si>
+    <t>0x101</t>
+  </si>
+  <si>
+    <t>0x102</t>
+  </si>
+  <si>
+    <t>0x200</t>
+  </si>
+  <si>
+    <t>0x300</t>
+  </si>
+  <si>
+    <t>0x400</t>
+  </si>
+  <si>
+    <t>0x500</t>
+  </si>
+  <si>
+    <t>0x600</t>
+  </si>
+  <si>
+    <t>0x700</t>
+  </si>
+  <si>
+    <t>0x800</t>
+  </si>
+  <si>
+    <t>0x900</t>
+  </si>
+  <si>
+    <t>0x901</t>
+  </si>
+  <si>
+    <t>0: Dont Care</t>
+  </si>
+  <si>
+    <t>Source ID</t>
+  </si>
+  <si>
+    <t>ESx, x: 0..n</t>
+  </si>
+  <si>
+    <t>0..y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used to calculate propagation delay. </t>
+  </si>
+  <si>
+    <t>Used to demonstrate a realistic data source from another communication channel</t>
+  </si>
+  <si>
+    <t>ms, s, us açıklama</t>
+  </si>
+  <si>
+    <t>m açıklama</t>
+  </si>
+  <si>
+    <t>[], () farkı açıklama</t>
+  </si>
+  <si>
+    <t>b, B açıklama</t>
+  </si>
+  <si>
+    <t>uniform açıklama</t>
+  </si>
+  <si>
+    <t>VL Queue size</t>
+  </si>
+  <si>
+    <t>ES Tx Tech Delay</t>
+  </si>
+  <si>
+    <t>ES Rx Tech Delay</t>
+  </si>
+  <si>
+    <t>Skew Max</t>
+  </si>
+  <si>
+    <t>Setting</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Datarate of source</t>
+  </si>
+  <si>
+    <t>between source and ES</t>
+  </si>
+  <si>
+    <t>Cable length</t>
+  </si>
+  <si>
+    <t>between source and ES[m]</t>
+  </si>
+  <si>
+    <t>VLID</t>
+  </si>
+  <si>
+    <t>[hex]</t>
+  </si>
+  <si>
+    <t>startTime</t>
+  </si>
+  <si>
+    <t>[us, ms, s]</t>
+  </si>
+  <si>
+    <t>stopTime</t>
+  </si>
+  <si>
+    <t>BAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (B)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rho </t>
+  </si>
+  <si>
+    <t>[bps, Mbps]</t>
+  </si>
+  <si>
+    <t>sigma</t>
+  </si>
+  <si>
+    <t>(b)</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>0.8ms</t>
+  </si>
+  <si>
+    <t>0.4ms</t>
+  </si>
+  <si>
+    <t>Payload Length</t>
+  </si>
+  <si>
+    <t>Delta Payload Length</t>
+  </si>
+  <si>
+    <t>Delta Period</t>
+  </si>
+  <si>
+    <t>End System</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,16 +397,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -193,14 +428,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,15 +789,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF69AB4-52F8-472A-9D5A-F167AD55A233}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -533,21 +807,92 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -555,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599FF63A-B559-42D2-99F2-9F8D52FECC3F}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,4 +1015,744 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B34407CB-7AC4-4FA3-8C80-BE9BE31A51C3}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView topLeftCell="BD1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="9">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{570773CE-9739-4C1A-9F1C-7A7BF1E7D7C1}">
+  <dimension ref="A1:N20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" activeCellId="1" sqref="A14 B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.6640625" style="12" customWidth="1"/>
+    <col min="11" max="12" width="13.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="12">
+        <v>0</v>
+      </c>
+      <c r="C2" s="12">
+        <v>0</v>
+      </c>
+      <c r="D2" s="12">
+        <v>0</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="12">
+        <v>0</v>
+      </c>
+      <c r="K2" s="12">
+        <v>1183</v>
+      </c>
+      <c r="L2" s="12">
+        <v>0</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="12">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12">
+        <v>0</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="12">
+        <v>0</v>
+      </c>
+      <c r="K3" s="12">
+        <v>1183</v>
+      </c>
+      <c r="L3" s="12">
+        <v>0</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="12">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="12">
+        <v>2</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="12">
+        <v>0</v>
+      </c>
+      <c r="K4" s="12">
+        <v>1183</v>
+      </c>
+      <c r="L4" s="12">
+        <v>0</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="12">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="12">
+        <v>0</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="12">
+        <v>0</v>
+      </c>
+      <c r="K5" s="12">
+        <v>1183</v>
+      </c>
+      <c r="L5" s="12">
+        <v>0</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="12">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="12">
+        <v>0</v>
+      </c>
+      <c r="K6" s="12">
+        <v>1183</v>
+      </c>
+      <c r="L6" s="12">
+        <v>0</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="12">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="12">
+        <v>0</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="12">
+        <v>0</v>
+      </c>
+      <c r="K7" s="12">
+        <v>1183</v>
+      </c>
+      <c r="L7" s="12">
+        <v>0</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="12">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="12">
+        <v>0</v>
+      </c>
+      <c r="C8" s="12">
+        <v>4125000</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="12">
+        <v>0</v>
+      </c>
+      <c r="K8" s="12">
+        <v>1183</v>
+      </c>
+      <c r="L8" s="12">
+        <v>100</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" s="12">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="12">
+        <v>0</v>
+      </c>
+      <c r="C9" s="12">
+        <v>0</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="12">
+        <v>0</v>
+      </c>
+      <c r="K9" s="12">
+        <v>1183</v>
+      </c>
+      <c r="L9" s="12">
+        <v>0</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="12">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="12">
+        <v>0</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0</v>
+      </c>
+      <c r="D10" s="12">
+        <v>0</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="K10" s="12">
+        <v>1183</v>
+      </c>
+      <c r="L10" s="12">
+        <v>0</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="12">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="12">
+        <v>0</v>
+      </c>
+      <c r="C11" s="12">
+        <v>0</v>
+      </c>
+      <c r="D11" s="12">
+        <v>0</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="12">
+        <v>0</v>
+      </c>
+      <c r="K11" s="12">
+        <v>1183</v>
+      </c>
+      <c r="L11" s="12">
+        <v>0</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" s="12">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="12">
+        <v>1183</v>
+      </c>
+      <c r="L12" s="12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" s="12">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="12">
+        <v>1</v>
+      </c>
+      <c r="C13" s="12">
+        <v>0</v>
+      </c>
+      <c r="D13" s="12">
+        <v>0</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="12">
+        <v>0</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="12">
+        <v>0</v>
+      </c>
+      <c r="K13" s="12">
+        <v>1183</v>
+      </c>
+      <c r="L13" s="12">
+        <v>0</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" s="12">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C18" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="M20" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="N20" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Progress in sheet3 parse
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\Github\ANCAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E6990E-1407-4320-8A02-F89DD6D6EE5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC847E71-B7BC-4505-B05F-BBE627E10CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13968" yWindow="492" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="3" xr2:uid="{60116E78-B1B7-4F11-A25A-D1AE9DCDD0BC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{60116E78-B1B7-4F11-A25A-D1AE9DCDD0BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="92">
   <si>
     <t>ES1</t>
   </si>
@@ -1106,7 +1106,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" activeCellId="1" sqref="A14 B15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1180,7 +1180,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>41</v>
@@ -1224,7 +1224,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>42</v>
@@ -1268,7 +1268,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>43</v>
@@ -1312,7 +1312,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>44</v>
@@ -1356,7 +1356,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>45</v>
@@ -1400,7 +1400,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="12">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>46</v>
@@ -1443,8 +1443,8 @@
       <c r="C8" s="12">
         <v>4125000</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>30</v>
+      <c r="D8" s="12">
+        <v>7</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>47</v>
@@ -1488,7 +1488,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="12">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>48</v>
@@ -1532,7 +1532,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="12">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>49</v>
@@ -1576,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>50</v>
@@ -1620,7 +1620,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="12">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>51</v>
@@ -1664,7 +1664,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="12">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>52</v>
@@ -1695,6 +1695,50 @@
       </c>
       <c r="N13" s="12">
         <v>15000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="12">
+        <v>0</v>
+      </c>
+      <c r="B17" s="12">
+        <v>1</v>
+      </c>
+      <c r="C17" s="12">
+        <v>2</v>
+      </c>
+      <c r="D17" s="12">
+        <v>3</v>
+      </c>
+      <c r="E17" s="12">
+        <v>4</v>
+      </c>
+      <c r="F17" s="12">
+        <v>5</v>
+      </c>
+      <c r="G17" s="12">
+        <v>6</v>
+      </c>
+      <c r="H17" s="12">
+        <v>7</v>
+      </c>
+      <c r="I17" s="12">
+        <v>8</v>
+      </c>
+      <c r="J17" s="12">
+        <v>9</v>
+      </c>
+      <c r="K17" s="12">
+        <v>10</v>
+      </c>
+      <c r="L17" s="12">
+        <v>11</v>
+      </c>
+      <c r="M17" s="12">
+        <v>12</v>
+      </c>
+      <c r="N17" s="12">
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:14" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Message set(end system info is done!!)
messageCount is missing. Will be added
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\Github\ANCAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC847E71-B7BC-4505-B05F-BBE627E10CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F25732-885C-4311-AEBC-5BFB1F0BC5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{60116E78-B1B7-4F11-A25A-D1AE9DCDD0BC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{60116E78-B1B7-4F11-A25A-D1AE9DCDD0BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="94">
   <si>
     <t>ES1</t>
   </si>
@@ -360,6 +360,12 @@
   </si>
   <si>
     <t>End System</t>
+  </si>
+  <si>
+    <t>ES10</t>
+  </si>
+  <si>
+    <t>0x0</t>
   </si>
 </sst>
 </file>
@@ -900,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599FF63A-B559-42D2-99F2-9F8D52FECC3F}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="A14:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1021,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B34407CB-7AC4-4FA3-8C80-BE9BE31A51C3}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView topLeftCell="BD1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1105,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{570773CE-9739-4C1A-9F1C-7A7BF1E7D7C1}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1697,6 +1703,50 @@
         <v>15000</v>
       </c>
     </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="12">
+        <v>1</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0</v>
+      </c>
+      <c r="D14" s="12">
+        <v>13</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="12">
+        <v>0</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="12">
+        <v>0</v>
+      </c>
+      <c r="K14" s="12">
+        <v>1183</v>
+      </c>
+      <c r="L14" s="12">
+        <v>0</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" s="12">
+        <v>15000</v>
+      </c>
+    </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>0</v>

</xml_diff>

<commit_message>
ANCAT is updated according to the new excel format
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\Github\ANCAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6D5606-887E-4DD4-95C2-43CE046218AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7AA826-4AD6-405D-AA60-634B04EAEB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{60116E78-B1B7-4F11-A25A-D1AE9DCDD0BC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{60116E78-B1B7-4F11-A25A-D1AE9DCDD0BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
     <sheet name="Topology" sheetId="1" r:id="rId2"/>
     <sheet name="Settings" sheetId="3" r:id="rId3"/>
     <sheet name="Message Set" sheetId="6" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="90">
   <si>
     <t>ES1</t>
   </si>
@@ -303,9 +302,6 @@
     <t>Delta Period</t>
   </si>
   <si>
-    <t>End System</t>
-  </si>
-  <si>
     <t>Define End Systems with ESx, x: 0..n (Es's shall be named without skipping any number: ES0, ES1, ES2..)</t>
   </si>
   <si>
@@ -330,9 +326,6 @@
     <t>partition ID</t>
   </si>
   <si>
-    <t>destination Ids</t>
-  </si>
-  <si>
     <t>0x3</t>
   </si>
   <si>
@@ -348,25 +341,19 @@
     <t>0x6</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>SW0-&gt;SW2-&gt;</t>
-  </si>
-  <si>
-    <t>SW1-&gt;SW2-&gt;SW3-&gt;</t>
-  </si>
-  <si>
     <t>Destination ES</t>
   </si>
   <si>
     <t>Source ES</t>
   </si>
   <si>
-    <t>ES5, ES6</t>
-  </si>
-  <si>
     <t>[hex], unique</t>
+  </si>
+  <si>
+    <t>source ve destination isimleri ES1,ES2 şeklinde olcak. Sadece virgül, var boşluk yok</t>
+  </si>
+  <si>
+    <t>0x10</t>
   </si>
 </sst>
 </file>
@@ -800,7 +787,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF69AB4-52F8-472A-9D5A-F167AD55A233}">
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
@@ -828,7 +815,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
@@ -843,7 +830,7 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
@@ -914,7 +901,12 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -925,549 +917,184 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599FF63A-B559-42D2-99F2-9F8D52FECC3F}">
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N7"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="8.88671875" style="13"/>
-    <col min="11" max="11" width="10.77734375" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.21875" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.44140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="13"/>
+    <col min="1" max="1" width="6" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="8.88671875" style="13"/>
+    <col min="8" max="8" width="10.77734375" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.21875" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>15</v>
+      </c>
       <c r="B1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>80</v>
-      </c>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
       <c r="M1" s="12"/>
-      <c r="N1" s="12" t="s">
-        <v>81</v>
-      </c>
+      <c r="N1" s="12"/>
       <c r="O1" s="12"/>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="12"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
-        <v>0</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="11">
-        <v>0</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" s="11">
-        <v>5</v>
-      </c>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11">
-        <v>7</v>
-      </c>
-      <c r="S2" s="11"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
-        <v>1</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="L3" s="11">
-        <v>10</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="P3" s="11">
-        <v>5</v>
-      </c>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11">
-        <v>7</v>
-      </c>
-      <c r="S3" s="11"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
-        <v>2</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="L4" s="11">
-        <v>20</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="N4" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="P4" s="11">
-        <v>5</v>
-      </c>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11">
-        <v>8</v>
-      </c>
-      <c r="S4" s="11"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
-        <v>3</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="L5" s="11">
-        <v>30</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="N5" s="13" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="Q5" s="11">
-        <v>6</v>
-      </c>
-      <c r="R5" s="11">
-        <v>9</v>
-      </c>
-      <c r="S5" s="11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
-        <v>4</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="L6" s="11">
-        <v>40</v>
-      </c>
-      <c r="M6" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="N6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q6" s="11">
-        <v>6</v>
-      </c>
-      <c r="R6" s="11">
-        <v>9</v>
-      </c>
-      <c r="S6" s="11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B7" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="13">
-        <v>5</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="L7" s="11">
-        <v>50</v>
-      </c>
-      <c r="M7" s="13" t="s">
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B8" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="13">
-        <v>6</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="L8" s="11">
-        <v>60</v>
-      </c>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B9" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="13">
-        <v>7</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="L9" s="11">
-        <v>70</v>
-      </c>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B10" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="13">
-        <v>8</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="L10" s="11">
-        <v>80</v>
-      </c>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B11" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="13">
-        <v>9</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B12" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B13" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="13">
-        <v>11</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="K13" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="L13" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="H14" s="13">
-        <v>0</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="K14" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="L14" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="H15" s="13">
-        <v>1</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="J15" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="K15" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="L15" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="H16" s="13">
-        <v>2</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="J16" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="K16" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="L16" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H17" s="13">
-        <v>3</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="J17" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="K17" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="L17" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H18" s="13">
-        <v>4</v>
-      </c>
-      <c r="I18" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="J18" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="K18" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="L18" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H19" s="13">
-        <v>5</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="J19" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="K19" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="L19" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H20" s="13">
-        <v>6</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="J20" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="K20" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="L20" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H21" s="13">
-        <v>7</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="J21" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="K21" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="L21" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H22" s="13">
-        <v>8</v>
-      </c>
-      <c r="I22" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="J22" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="K22" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L22" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H23" s="13">
-        <v>9</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="J23" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="K23" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="L23" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H24" s="13">
-        <v>10</v>
-      </c>
-      <c r="I24" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="J24" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="K24" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="L24" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="I25" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="J25" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="K25" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="L25" s="13" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1483,7 +1110,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1564,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{570773CE-9739-4C1A-9F1C-7A7BF1E7D7C1}">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1589,16 +1216,16 @@
   <sheetData>
     <row r="1" spans="1:15" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>59</v>
@@ -1639,10 +1266,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>92</v>
+        <v>9</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D2" s="11">
         <v>0</v>
@@ -1678,24 +1305,24 @@
         <v>0</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D3" s="11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>31</v>
@@ -1725,24 +1352,24 @@
         <v>0</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D4" s="11">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>31</v>
@@ -1772,24 +1399,24 @@
         <v>0</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D5" s="11">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>31</v>
@@ -1819,24 +1446,24 @@
         <v>0</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D6" s="11">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>31</v>
@@ -1854,7 +1481,7 @@
         <v>1183</v>
       </c>
       <c r="K6" s="11">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="L6" s="11" t="s">
         <v>27</v>
@@ -1862,28 +1489,28 @@
       <c r="M6" s="11">
         <v>15000</v>
       </c>
-      <c r="N6" s="11" t="s">
-        <v>77</v>
+      <c r="N6" s="11">
+        <v>0</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D7" s="11">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>31</v>
@@ -1913,73 +1540,214 @@
         <v>0</v>
       </c>
       <c r="O7" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="11">
+        <v>40</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="11">
+        <v>0</v>
+      </c>
+      <c r="J8" s="11">
+        <v>1183</v>
+      </c>
+      <c r="K8" s="11">
+        <v>100</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="11">
+        <v>15000</v>
+      </c>
+      <c r="N8" s="11" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="N10" s="9" t="s">
+      <c r="O8" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="11">
+        <v>40</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0</v>
+      </c>
+      <c r="J9" s="11">
+        <v>1183</v>
+      </c>
+      <c r="K9" s="11">
+        <v>100</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" s="11">
+        <v>15000</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="11">
+        <v>50</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="11">
+        <v>0</v>
+      </c>
+      <c r="J10" s="11">
+        <v>1183</v>
+      </c>
+      <c r="K10" s="11">
+        <v>0</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="11">
+        <v>15000</v>
+      </c>
+      <c r="N10" s="11">
+        <v>0</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="N13" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="O10" s="9" t="s">
+      <c r="O13" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+    <row r="14" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="N11" s="10" t="s">
+      <c r="N14" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="O11" s="10" t="s">
+      <c r="O14" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E12" s="10" t="s">
+    <row r="15" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G15" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J15" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="K12" s="10" t="s">
+      <c r="K15" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="L15" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="M12" s="10" t="s">
+      <c r="M15" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="N12" s="10" t="s">
+      <c r="N15" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="O12" s="10" t="s">
+      <c r="O15" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C19" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C20" s="11">
         <v>2</v>
       </c>
     </row>
@@ -1987,16 +1755,4 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEA44F9-3ECF-45F1-A65B-75DA2C72143E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Latest tweaks and DONE!(Preprocessing)
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ozerg\Documents\GitHub\ANCAT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\Github\ANCAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFF1BD6-EE31-4B4B-8AC9-556062484A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCD742B-FC65-4D43-B4AA-3E1C832C2535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{60116E78-B1B7-4F11-A25A-D1AE9DCDD0BC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{60116E78-B1B7-4F11-A25A-D1AE9DCDD0BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -82,12 +82,6 @@
   </si>
   <si>
     <t>Define Switches with SWx, x: 0..n</t>
-  </si>
-  <si>
-    <t>Entry</t>
-  </si>
-  <si>
-    <t>Exit</t>
   </si>
   <si>
     <t xml:space="preserve">! Her bağlantı bir kere </t>
@@ -368,6 +362,12 @@
   </si>
   <si>
     <t>ES5, ES7, ES8</t>
+  </si>
+  <si>
+    <t>End1</t>
+  </si>
+  <si>
+    <t>End2</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -487,6 +487,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,120 +819,120 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="85.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="85.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -933,29 +945,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599FF63A-B559-42D2-99F2-9F8D52FECC3F}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="8.85546875" style="13"/>
-    <col min="8" max="8" width="10.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="8.88671875" style="13"/>
+    <col min="8" max="8" width="10.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" style="13" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="13"/>
+    <col min="13" max="16384" width="8.88671875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
@@ -967,7 +979,7 @@
       <c r="O1" s="12"/>
       <c r="P1" s="12"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
@@ -981,7 +993,7 @@
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -995,7 +1007,7 @@
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
@@ -1009,7 +1021,7 @@
       <c r="O4" s="11"/>
       <c r="P4" s="11"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>7</v>
       </c>
@@ -1022,7 +1034,7 @@
       <c r="O5" s="11"/>
       <c r="P5" s="11"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>8</v>
       </c>
@@ -1035,7 +1047,7 @@
       <c r="O6" s="11"/>
       <c r="P6" s="11"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>5</v>
       </c>
@@ -1049,7 +1061,7 @@
       <c r="O7" s="11"/>
       <c r="P7" s="11"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
@@ -1062,7 +1074,7 @@
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>6</v>
       </c>
@@ -1075,7 +1087,7 @@
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>6</v>
       </c>
@@ -1088,7 +1100,7 @@
       <c r="K10" s="11"/>
       <c r="L10" s="11"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>6</v>
       </c>
@@ -1096,7 +1108,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>11</v>
       </c>
@@ -1104,7 +1116,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>11</v>
       </c>
@@ -1127,71 +1139,71 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="8" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="B5" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="B7" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B8" s="8">
         <v>1000</v>
@@ -1207,98 +1219,98 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{570773CE-9739-4C1A-9F1C-7A7BF1E7D7C1}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.7109375" style="11" customWidth="1"/>
-    <col min="10" max="11" width="13.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.6640625" style="11" customWidth="1"/>
+    <col min="10" max="11" width="13.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" style="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="11"/>
+    <col min="14" max="14" width="27.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>79</v>
+        <v>56</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>77</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="G1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="N1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="11">
+        <v>72</v>
+      </c>
+      <c r="D2" s="16">
         <v>0</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>33</v>
-      </c>
       <c r="H2" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I2" s="11">
         <v>0</v>
@@ -1310,7 +1322,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M2" s="11">
         <v>15000</v>
@@ -1319,10 +1331,10 @@
         <v>0</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
@@ -1330,22 +1342,22 @@
         <v>9</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="11">
+        <v>87</v>
+      </c>
+      <c r="D3" s="16">
         <v>0</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>33</v>
-      </c>
       <c r="H3" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I3" s="11">
         <v>0</v>
@@ -1357,7 +1369,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M3" s="11">
         <v>15000</v>
@@ -1366,10 +1378,10 @@
         <v>0</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
@@ -1377,22 +1389,22 @@
         <v>9</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="11">
+        <v>88</v>
+      </c>
+      <c r="D4" s="16">
         <v>0</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>33</v>
-      </c>
       <c r="H4" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I4" s="11">
         <v>0</v>
@@ -1404,7 +1416,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M4" s="11">
         <v>15000</v>
@@ -1413,10 +1425,10 @@
         <v>0</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>0</v>
       </c>
@@ -1424,22 +1436,22 @@
         <v>9</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="11">
+        <v>79</v>
+      </c>
+      <c r="D5" s="16">
         <v>10</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>33</v>
-      </c>
       <c r="H5" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I5" s="11">
         <v>0</v>
@@ -1451,7 +1463,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M5" s="11">
         <v>15000</v>
@@ -1460,10 +1472,10 @@
         <v>0</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>2</v>
       </c>
@@ -1471,22 +1483,22 @@
         <v>10</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="11">
+        <v>78</v>
+      </c>
+      <c r="D6" s="16">
         <v>20</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>33</v>
-      </c>
       <c r="H6" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I6" s="11">
         <v>0</v>
@@ -1498,7 +1510,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M6" s="11">
         <v>15000</v>
@@ -1507,33 +1519,33 @@
         <v>0</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" s="11">
+        <v>80</v>
+      </c>
+      <c r="D7" s="16">
         <v>30</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>33</v>
-      </c>
       <c r="H7" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I7" s="11">
         <v>0</v>
@@ -1545,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M7" s="11">
         <v>15000</v>
@@ -1554,10 +1566,10 @@
         <v>0</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>8</v>
       </c>
@@ -1565,22 +1577,22 @@
         <v>12</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="D8" s="11">
+        <v>81</v>
+      </c>
+      <c r="D8" s="16">
         <v>40</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>33</v>
-      </c>
       <c r="H8" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I8" s="11">
         <v>0</v>
@@ -1592,42 +1604,42 @@
         <v>100</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M8" s="11">
         <v>15000</v>
       </c>
       <c r="N8" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" s="11">
+        <v>89</v>
+      </c>
+      <c r="D9" s="16">
         <v>40</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>33</v>
-      </c>
       <c r="H9" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I9" s="11">
         <v>0</v>
@@ -1639,19 +1651,19 @@
         <v>100</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M9" s="11">
         <v>15000</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>9</v>
       </c>
@@ -1659,22 +1671,22 @@
         <v>13</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="11">
+        <v>82</v>
+      </c>
+      <c r="D10" s="16">
         <v>50</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="11" t="s">
-        <v>33</v>
-      </c>
       <c r="H10" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I10" s="11">
         <v>0</v>
@@ -1686,7 +1698,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M10" s="11">
         <v>15000</v>
@@ -1695,61 +1707,64 @@
         <v>0</v>
       </c>
       <c r="O10" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D13" s="17"/>
       <c r="N13" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>40</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D14" s="18"/>
       <c r="N14" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="O14" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C15" s="10" t="s">
-        <v>87</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="D15" s="18"/>
       <c r="E15" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J15" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="L15" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="K15" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="L15" s="10" t="s">
+      <c r="M15" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="M15" s="10" t="s">
-        <v>67</v>
-      </c>
       <c r="N15" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="O15" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="O15" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>4</v>
       </c>
@@ -1757,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>4</v>
       </c>

</xml_diff>